<commit_message>
feat: Implement sentiment analysis and takeaway generation with a new frontend UI.
</commit_message>
<xml_diff>
--- a/backend/data/comment.xlsx
+++ b/backend/data/comment.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:A53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,14 +485,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>this is test message</t>
+          <t>hlo sir</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>hlo sir</t>
+          <t>Wow that's great</t>
         </is>
       </c>
     </row>
@@ -772,26 +772,33 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>hi</t>
+          <t>this is test message</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>if any update will be publish contact me 9818019048</t>
+          <t>hi</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>can i get the other comment too</t>
+          <t>if any update will be publish contact me 9818019048</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
+        <is>
+          <t>can i get the other comment too</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
         <is>
           <t>Hi 👋, 98777377273</t>
         </is>

</xml_diff>

<commit_message>
Feat(app):add frontend and backend logic
</commit_message>
<xml_diff>
--- a/backend/data/comment.xlsx
+++ b/backend/data/comment.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,315 +492,651 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Wow that's great</t>
+          <t>I don’t think I would buy this.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>I don’t trust AI wellness devices.</t>
+          <t>Too many features can be confusing.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Probably another over-priced gadget.</t>
+          <t>Not convinced it’s really useful.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Seems too good to be true.</t>
+          <t>Sounds like marketing hype.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>I don’t think this will work as advertised.</t>
+          <t>I doubt it will give accurate advice.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Is it rechargeable or battery powered?</t>
+          <t>Might be hard for older people.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>When will it be available in Nepal?</t>
+          <t>I prefer simple fitness bands.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Does it need a mobile app to work?</t>
+          <t>Probably needs too many subscriptions.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>What is the price range?</t>
+          <t>I don’t feel comfortable sharing health data.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>I’m excited for the launch!</t>
+          <t>This looks complicated to use.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Brilliant concept and design.</t>
+          <t>Is there a demo video?</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Health tracking plus motivation — love it.</t>
+          <t>Can it be used while sleeping?</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>This would be great for students too.</t>
+          <t>What is the return policy?</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GlowMate seems super helpful.</t>
+          <t>Is international shipping available?</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Such a smart invention!</t>
+          <t>Does it come with a warranty?</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Huge fan of wellness tech — this looks perfect.</t>
+          <t>Can multiple users use one device?</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>This is exactly what modern life needs.</t>
+          <t>How long does the battery last?</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Great product for mental wellness.</t>
+          <t>Does it support Android and iOS?</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>I love the mood-boosting concept.</t>
+          <t>Is it available in black color?</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Looks simple yet powerful.</t>
+          <t>What phones are compatible with it?</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>This could improve daily life.</t>
+          <t>Looks like a thoughtful invention.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Amazing technology packed into a small device.</t>
+          <t>Seems well designed.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Would love to see this in stores soon.</t>
+          <t>Pocket wellness coach — nice!</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Very impressive product idea.</t>
+          <t>This could improve productivity.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>I struggle with stress — this would help a lot.</t>
+          <t>I like the stress monitoring feature.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Pocket-sized wellness coach? Brilliant!</t>
+          <t>Great thinking behind this product.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Definitely recommending this to my friends.</t>
+          <t>Makes self-care easier.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>So innovative and useful.</t>
+          <t>This is such a smart innovation.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>This feels like the future of healthcare.</t>
+          <t>Looks very user-friendly.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>The sleep improvement feature is awesome.</t>
+          <t>Wellness tech done right.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Can’t wait to try GlowMate!</t>
+          <t>Could be helpful for remote workers.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Perfect for working professionals.</t>
+          <t>Love the personal assistant feel.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>This could help so many people.</t>
+          <t>A smart solution for modern stress.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>I really like the AI wellness feature.</t>
+          <t>Helps people focus on their mental health.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Great idea for people with busy schedules.</t>
+          <t>Good product for personal wellness.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Looks like a life-changing device.</t>
+          <t>Feels modern and useful.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Would buy this instantly!</t>
+          <t>Would love to test this.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Love the concept — very futuristic.</t>
+          <t>I like the sleek gadget idea.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Finally a smart wellness gadget that actually makes sense.</t>
+          <t>This could reduce daily anxiety.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Interesting concept, curious to review</t>
+          <t>A nice blend of tech and health.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>this is test message</t>
+          <t>Sounds like a digital wellness buddy.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>hi</t>
+          <t>Smart reminders are a great touch.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>if any update will be publish contact me 9818019048</t>
+          <t>I’d gift this to my parents.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>can i get the other comment too</t>
+          <t>Looks super handy to carry around.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Hi 👋, 98777377273</t>
+          <t>Perfect for people working long hours.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>I like the idea of mood monitoring.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>This could really help people who forget self-care.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Wellness made simple — nice concept.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Love how compact yet powerful it sounds.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>This gadget feels very premium and thoughtful.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Wow that's great</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>I don’t trust AI wellness devices.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Probably another over-priced gadget.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Seems too good to be true.</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>I don’t think this will work as advertised.</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Is it rechargeable or battery powered?</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>When will it be available in Nepal?</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Does it need a mobile app to work?</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>What is the price range?</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>I’m excited for the launch!</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Brilliant concept and design.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Health tracking plus motivation — love it.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>This would be great for students too.</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>GlowMate seems super helpful.</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Such a smart invention!</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Huge fan of wellness tech — this looks perfect.</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>This is exactly what modern life needs.</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Great product for mental wellness.</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>I love the mood-boosting concept.</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Looks simple yet powerful.</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>This could improve daily life.</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Amazing technology packed into a small device.</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Would love to see this in stores soon.</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Very impressive product idea.</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>I struggle with stress — this would help a lot.</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Pocket-sized wellness coach? Brilliant!</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Definitely recommending this to my friends.</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>So innovative and useful.</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>This feels like the future of healthcare.</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>The sleep improvement feature is awesome.</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Can’t wait to try GlowMate!</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Perfect for working professionals.</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>This could help so many people.</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>I really like the AI wellness feature.</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Great idea for people with busy schedules.</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Looks like a life-changing device.</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Would buy this instantly!</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Love the concept — very futuristic.</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Finally a smart wellness gadget that actually makes sense.</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Interesting concept, curious to review</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>this is test message</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>if any update will be publish contact me 9818019048</t>
         </is>
       </c>
     </row>

</xml_diff>